<commit_message>
just commit  Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/300190_维尔利/维尔利.xlsx
+++ b/300190_维尔利/维尔利.xlsx
@@ -5,19 +5,20 @@
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/external/doc/personal/stock/300190_维尔利/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/external/git/stock_learn/300190_维尔利/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="3900" windowWidth="25600" windowHeight="14780"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14780" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="自由现金流" sheetId="2" r:id="rId2"/>
     <sheet name="工作表2" sheetId="3" r:id="rId3"/>
-    <sheet name="现金流净利润比" sheetId="4" r:id="rId4"/>
-    <sheet name="应收" sheetId="7" r:id="rId5"/>
-    <sheet name="存货" sheetId="6" r:id="rId6"/>
+    <sheet name="估值" sheetId="8" r:id="rId4"/>
+    <sheet name="现金流净利润比" sheetId="4" r:id="rId5"/>
+    <sheet name="应收" sheetId="7" r:id="rId6"/>
+    <sheet name="存货" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="119">
   <si>
     <t>年份</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1160,6 +1161,80 @@
   </si>
   <si>
     <t>资产利用率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经营活动产生的现金流量净额</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始净利润</t>
+    <rPh sb="0" eb="1">
+      <t>chu'shi</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>jing'li'run</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最终估值</t>
+    <rPh sb="0" eb="1">
+      <t>zui'zhong</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>gu'zhi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预估净利润</t>
+    <rPh sb="0" eb="1">
+      <t>yu'gu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>jinl'gi'run</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>折现价值</t>
+    <rPh sb="0" eb="1">
+      <t>zhe'xian</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>jia'zhi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>折扣估值</t>
+    <rPh sb="0" eb="1">
+      <t>zhe'kou</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>gu'zhi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>符合增长</t>
+    <rPh sb="0" eb="1">
+      <t>fu'he</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>zeng'zhang</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接盘价格</t>
+    <rPh sb="0" eb="1">
+      <t>jie'pan</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>jia'ge</t>
+    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1233,7 +1308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1259,6 +1334,18 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1547,7 +1634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:W111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+    <sheetView topLeftCell="A80" workbookViewId="0">
       <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
@@ -3550,14 +3637,14 @@
         <v>1249415004.1199999</v>
       </c>
       <c r="E83" s="7">
-        <f t="shared" ref="E83:E92" si="16">C83-D83</f>
+        <f t="shared" ref="E83:E90" si="16">C83-D83</f>
         <v>168350371.49000001</v>
       </c>
       <c r="F83" s="5">
         <v>186731142.05000001</v>
       </c>
       <c r="G83" s="2">
-        <f t="shared" ref="G83:G92" si="17">F83/C83</f>
+        <f t="shared" ref="G83:G90" si="17">F83/C83</f>
         <v>0.13170807050472516</v>
       </c>
       <c r="H83" s="1">
@@ -5003,10 +5090,394 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:N20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" customWidth="1"/>
+    <col min="10" max="10" width="15.5" customWidth="1"/>
+    <col min="11" max="11" width="13.5" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="10">
+        <v>2009</v>
+      </c>
+      <c r="C2" s="10">
+        <v>2010</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2011</v>
+      </c>
+      <c r="E2" s="10">
+        <v>2012</v>
+      </c>
+      <c r="F2" s="10">
+        <v>2013</v>
+      </c>
+      <c r="G2" s="10">
+        <v>2014</v>
+      </c>
+      <c r="H2" s="10">
+        <v>2015</v>
+      </c>
+      <c r="I2" s="10">
+        <v>2016</v>
+      </c>
+      <c r="J2" s="10">
+        <v>2017</v>
+      </c>
+      <c r="K2" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="9">
+        <v>45143297.100000001</v>
+      </c>
+      <c r="D3" s="9">
+        <v>47735376.670000002</v>
+      </c>
+      <c r="E3" s="9">
+        <v>68000398.879999995</v>
+      </c>
+      <c r="F3" s="9">
+        <v>28881580</v>
+      </c>
+      <c r="G3" s="9">
+        <v>96069481.920000002</v>
+      </c>
+      <c r="H3" s="9">
+        <v>120559675.81</v>
+      </c>
+      <c r="I3" s="9">
+        <v>92753424.450000003</v>
+      </c>
+      <c r="J3" s="9">
+        <v>138703129.69</v>
+      </c>
+      <c r="K3" s="9">
+        <v>232366860.28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="2" t="e">
+        <f>(C3-B3)/B3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:K4" si="0">(D3-C3)/C3</f>
+        <v>5.7418924547272383E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.42452838175121899</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.57527337374936294</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>2.3263236263390024</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.2549216816886109</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.23064305020048476</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.49539632107890325</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.67528202715639818</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5">
+        <f>(K3-C3)/C3/9</f>
+        <v>0.46081299921513952</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="20">
+        <f>K3*0.27</f>
+        <v>62739052.275600001</v>
+      </c>
+      <c r="B8" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="C8" s="19">
+        <v>15</v>
+      </c>
+      <c r="D8" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="E8" s="19">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="19"/>
+      <c r="B10" s="21">
+        <v>0.18</v>
+      </c>
+      <c r="C10" s="21">
+        <v>0.18</v>
+      </c>
+      <c r="D10" s="21">
+        <v>0.18</v>
+      </c>
+      <c r="E10" s="21">
+        <v>0.18</v>
+      </c>
+      <c r="F10" s="21">
+        <v>0.18</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="19">
+        <v>2019</v>
+      </c>
+      <c r="C11" s="19">
+        <v>2020</v>
+      </c>
+      <c r="D11" s="19">
+        <v>2021</v>
+      </c>
+      <c r="E11" s="19">
+        <v>2022</v>
+      </c>
+      <c r="F11" s="19">
+        <v>2023</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="22">
+        <f>A8*(1+D8)</f>
+        <v>81560767.958279997</v>
+      </c>
+      <c r="C12" s="22">
+        <f>B12*(1+D8)</f>
+        <v>106028998.345764</v>
+      </c>
+      <c r="D12" s="22">
+        <f>C12*(1+D8)</f>
+        <v>137837697.84949321</v>
+      </c>
+      <c r="E12" s="22">
+        <f>D12*(1+D8)</f>
+        <v>179189007.20434117</v>
+      </c>
+      <c r="F12" s="22">
+        <f>E12*(1+D8)</f>
+        <v>232945709.36564353</v>
+      </c>
+      <c r="G12" s="22">
+        <f>F12*C8</f>
+        <v>3494185640.484653</v>
+      </c>
+      <c r="H12" s="19"/>
+      <c r="M12">
+        <v>2018</v>
+      </c>
+      <c r="N12" s="9">
+        <v>232366860.28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="20">
+        <f>B12/(1+B8)</f>
+        <v>77676921.86502856</v>
+      </c>
+      <c r="C13" s="20">
+        <f>C12/(1+B8)^2</f>
+        <v>96171427.070987746</v>
+      </c>
+      <c r="D13" s="20">
+        <f>D12/(1+B8)^3</f>
+        <v>119069385.8974134</v>
+      </c>
+      <c r="E13" s="20">
+        <f>E12/(1+B8)^4</f>
+        <v>147419239.68251187</v>
+      </c>
+      <c r="F13" s="20">
+        <f>F12/(1+B8)^5</f>
+        <v>182519058.65453848</v>
+      </c>
+      <c r="G13" s="20">
+        <f>G12/(1+B8)^4</f>
+        <v>2874675173.8089814</v>
+      </c>
+      <c r="H13" s="20">
+        <f>SUM(B13:G13)</f>
+        <v>3497531206.9794617</v>
+      </c>
+      <c r="M13">
+        <f>M12-1</f>
+        <v>2017</v>
+      </c>
+      <c r="N13" s="9">
+        <v>138703129.69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="19"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" s="20">
+        <f>H13*E8</f>
+        <v>5246296810.4691925</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ref="M14:M20" si="1">M13-1</f>
+        <v>2016</v>
+      </c>
+      <c r="N14" s="9">
+        <v>92753424.450000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>2015</v>
+      </c>
+      <c r="N15" s="9">
+        <v>120559675.81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>2014</v>
+      </c>
+      <c r="N16" s="9">
+        <v>96069481.920000002</v>
+      </c>
+    </row>
+    <row r="17" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>2013</v>
+      </c>
+      <c r="N17" s="9">
+        <v>28881580</v>
+      </c>
+    </row>
+    <row r="18" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>2012</v>
+      </c>
+      <c r="N18" s="9">
+        <v>68000398.879999995</v>
+      </c>
+    </row>
+    <row r="19" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>2011</v>
+      </c>
+      <c r="N19" s="9">
+        <v>47735376.670000002</v>
+      </c>
+    </row>
+    <row r="20" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>2010</v>
+      </c>
+      <c r="N20" s="9">
+        <v>45143297.100000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K13"/>
+      <selection activeCell="A4" sqref="A4:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5950,22 +6421,22 @@
       <c r="Z15" s="9"/>
     </row>
     <row r="16" spans="1:27" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
@@ -6044,7 +6515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6059,7 +6530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L13"/>
   <sheetViews>

</xml_diff>